<commit_message>
local test uploads 📂
</commit_message>
<xml_diff>
--- a/database/seeders/uploads/local/departments.xlsx
+++ b/database/seeders/uploads/local/departments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\raul\wowsbar\database\seeders\uploads\local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBA25C5-7938-430B-8D51-428454ACEC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9BF685-4CEF-4AF7-B619-309EFE485AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15270" yWindow="0" windowWidth="15540" windowHeight="18570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>